<commit_message>
CHP study reports update
</commit_message>
<xml_diff>
--- a/Reports/CHP-study/chp-conveyors.xlsx
+++ b/Reports/CHP-study/chp-conveyors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CHP\Reports\CHP-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195F7A86-39B4-4C8B-B654-849F34FE4E7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78B538B-7EEE-4979-9C08-807DA7AD17B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
   <si>
     <t>CV 1.1</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>BELT LENGTH (m)</t>
+  </si>
+  <si>
+    <t>EP Series</t>
   </si>
 </sst>
 </file>
@@ -301,14 +304,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF0F0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -603,8 +599,8 @@
   </sheetPr>
   <dimension ref="B2:I24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I24"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,8 +1107,12 @@
       <c r="E21" s="2">
         <v>687</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="H21" s="2" t="s">
         <v>39</v>
       </c>
@@ -1133,8 +1133,12 @@
       <c r="E22" s="2">
         <v>74</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="H22" s="2" t="s">
         <v>39</v>
       </c>
@@ -1155,8 +1159,12 @@
       <c r="E23" s="2">
         <v>360</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="H23" s="2" t="s">
         <v>39</v>
       </c>
@@ -1177,8 +1185,12 @@
       <c r="E24" s="2">
         <v>410</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="F24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="H24" s="2" t="s">
         <v>39</v>
       </c>
@@ -1192,7 +1204,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B3:I24">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(B3),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>